<commit_message>
Inserindo 3 cenarios negativos
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/Massa.xlsx
+++ b/src/test/resources/Excel/Massa.xlsx
@@ -3,32 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E7764142-505C-4279-A7C1-F5F10F0D142A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{915CBFCB-CDB1-484A-A62D-874C932866D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="20760" windowHeight="14625" activeTab="1" xr2:uid="{42C517F9-3C2F-4E44-A03E-BA06A54FC42C}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="20850" windowHeight="15660" activeTab="1" xr2:uid="{42C517F9-3C2F-4E44-A03E-BA06A54FC42C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Cadastro" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:H18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Usuario</t>
   </si>
@@ -78,40 +72,52 @@
     <t>PostalCode</t>
   </si>
   <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Santo Andre</t>
+  </si>
+  <si>
+    <t>Rua Natal</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>rodrigo</t>
+  </si>
+  <si>
+    <t>rodrigo1@gmail.com</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
+  </si>
+  <si>
+    <t>Morais</t>
+  </si>
+  <si>
+    <t>+11953459465</t>
+  </si>
+  <si>
+    <t>+11990909898</t>
+  </si>
+  <si>
+    <t>09030600</t>
+  </si>
+  <si>
+    <t>09030601</t>
+  </si>
+  <si>
+    <t>VictorAlbano@gmail.com</t>
+  </si>
+  <si>
     <t>Victor</t>
   </si>
   <si>
     <t>Albano</t>
   </si>
   <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>Santo Andre</t>
-  </si>
-  <si>
-    <t>Rua Natal</t>
-  </si>
-  <si>
-    <t>SP</t>
-  </si>
-  <si>
-    <t>rodrigo</t>
-  </si>
-  <si>
-    <t>rodrigo1@gmail.com</t>
-  </si>
-  <si>
-    <t>Rodrigo</t>
-  </si>
-  <si>
-    <t>Morais</t>
-  </si>
-  <si>
-    <t>FernandesAlbano17</t>
-  </si>
-  <si>
-    <t>FernandesAlbano17@gmail.com</t>
+    <t>VictorAlbano17</t>
   </si>
 </sst>
 </file>
@@ -185,7 +191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -203,6 +209,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -523,7 +532,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +575,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,72 +631,72 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="5">
-        <v>11953459764</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="5">
-        <v>9030600</v>
+      <c r="K2" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="5">
-        <v>11990909898</v>
-      </c>
       <c r="G3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="5">
-        <v>9030601</v>
+      <c r="K3" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>